<commit_message>
coords now checks for recorded coordinates before calling API. Also lists client/driver names who did not get a confident set of coordinates back from the API.
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -559,34 +559,34 @@
   </sheetPr>
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="3" t="inlineStr">
         <is>
           <t>fName</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="3" t="inlineStr">
         <is>
           <t>lName</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="3" t="inlineStr">
         <is>
           <t>address</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="D1" s="3" t="inlineStr">
         <is>
           <t>lat</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="E1" s="3" t="inlineStr">
         <is>
           <t>long</t>
         </is>
@@ -608,6 +608,8 @@
           <t>543 osborne st</t>
         </is>
       </c>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -625,9 +627,11 @@
           <t>434 kimberly ave</t>
         </is>
       </c>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
getting API response. Need to start parsing response
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeremyklassen/Desktop/Proj/DriveScheduler/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A153D468-84F3-084B-85A4-422F2B7A09C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDE40C4E-3794-3240-B892-F6B861549B96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1700" yWindow="500" windowWidth="26720" windowHeight="16940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1700" yWindow="500" windowWidth="26720" windowHeight="16940" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="clients" sheetId="1" r:id="rId1"/>
@@ -18,12 +18,25 @@
     <sheet name="distances" sheetId="3" r:id="rId3"/>
     <sheet name="keys" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
   <si>
     <t>fName</t>
   </si>
@@ -76,12 +89,6 @@
     <t>434 kimberly ave</t>
   </si>
   <si>
-    <t>clientId</t>
-  </si>
-  <si>
-    <t>driverId</t>
-  </si>
-  <si>
     <t>distance</t>
   </si>
   <si>
@@ -98,13 +105,34 @@
   </si>
   <si>
     <t>96668959e23d9b614fcbe45b75e6eb61</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>Id1</t>
+  </si>
+  <si>
+    <t>Id2</t>
+  </si>
+  <si>
+    <t>API_KEY</t>
+  </si>
+  <si>
+    <t>db04e55a43e11768c3ba45fba5736975</t>
+  </si>
+  <si>
+    <t>API_ID</t>
+  </si>
+  <si>
+    <t>e4519f0a</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -122,6 +150,20 @@
       <b/>
       <sz val="12"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -159,12 +201,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -479,60 +523,294 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
+    <col min="1" max="1" width="54" customWidth="1"/>
     <col min="3" max="3" width="40.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:6">
+      <c r="A1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
+    <row r="2" spans="1:6">
+      <c r="A2" t="str">
+        <f>_xlfn.CONCAT(B2,C2)</f>
+        <v>jeremyklassen</v>
+      </c>
+      <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>49.885171999999997</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>-97.163939999999997</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
+    <row r="3" spans="1:6">
+      <c r="A3" t="str">
+        <f t="shared" ref="A3:A40" si="0">_xlfn.CONCAT(B3,C3)</f>
+        <v>timmytheKid</v>
+      </c>
+      <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
     </row>
   </sheetData>
@@ -542,49 +820,287 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="34.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:6">
+      <c r="A1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
+    <row r="2" spans="1:6">
+      <c r="A2" t="str">
+        <f>_xlfn.CONCAT(B2:C2)</f>
+        <v>maxmcbain</v>
+      </c>
+      <c r="B2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
+    <row r="3" spans="1:6">
+      <c r="A3" t="str">
+        <f t="shared" ref="A3:A40" si="0">_xlfn.CONCAT(B3:C3)</f>
+        <v>billybilborne</v>
+      </c>
+      <c r="B3" t="s">
         <v>14</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>15</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
     </row>
   </sheetData>
@@ -597,23 +1113,23 @@
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
         <v>17</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>18</v>
-      </c>
-      <c r="C1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -623,28 +1139,44 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Greedy algorithm is working
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeremyklassen/Desktop/Proj/DriveScheduler/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C476F9B9-7D64-6E40-B606-E5B8A4799C3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16B3E45C-6B10-9741-8757-2B4AEFFDC7DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1700" yWindow="500" windowWidth="26720" windowHeight="16940" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1700" yWindow="500" windowWidth="26720" windowHeight="16940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="clients" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="49">
   <si>
     <t>id</t>
   </si>
@@ -64,7 +64,7 @@
     <t>theKid</t>
   </si>
   <si>
-    <t>1254 Portage Ave, Winnipeg, MB R3G 0T6</t>
+    <t>1250 Portage Ave, Winnipeg, MB R3G 0T6</t>
   </si>
   <si>
     <t>johnnytheMan</t>
@@ -170,12 +170,6 @@
   </si>
   <si>
     <t>96668959e23d9b614fcbe45b75e6eb61</t>
-  </si>
-  <si>
-    <t>API_KEY</t>
-  </si>
-  <si>
-    <t>305f3e44-cb77-450e-bdd4-081a0aad601d</t>
   </si>
 </sst>
 </file>
@@ -564,9 +558,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <sheetData>
@@ -688,6 +684,46 @@
       </c>
       <c r="F6">
         <v>-97.189682000000005</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7">
+        <v>49.812044</v>
+      </c>
+      <c r="F7">
+        <v>-97.154775999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8">
+        <v>49.828966000000001</v>
+      </c>
+      <c r="F8">
+        <v>-97.053804</v>
       </c>
     </row>
   </sheetData>
@@ -697,9 +733,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:F6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <sheetData>
@@ -781,46 +819,6 @@
       </c>
       <c r="F4">
         <v>-97.094491000000005</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D5" t="s">
-        <v>40</v>
-      </c>
-      <c r="E5">
-        <v>49.812044</v>
-      </c>
-      <c r="F5">
-        <v>-97.154775999999998</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" t="s">
-        <v>41</v>
-      </c>
-      <c r="B6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E6">
-        <v>49.828966000000001</v>
-      </c>
-      <c r="F6">
-        <v>-97.053804</v>
       </c>
     </row>
   </sheetData>
@@ -832,7 +830,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <sheetData>
@@ -1225,15 +1223,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B7" sqref="B7:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>45</v>
       </c>
@@ -1241,7 +1239,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -1249,17 +1247,13 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="B7" s="2"/>
+      <c r="C7" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>